<commit_message>
commit updated alk TC02 flags
</commit_message>
<xml_diff>
--- a/RAS01-Pulse6/RAS1_Pulse6.xlsx
+++ b/RAS01-Pulse6/RAS1_Pulse6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/cloudstor/Shared/RAS_QCd_final_formatted/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/cloudstor/Shared/SOTS_Annual Reports/QC documentation/RAS QC/updated alk TCO2 flags/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDE09F4-EF0A-6C4A-BBB7-D5D64D88A981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF5D16F-8842-3848-B5B0-D5E694C80BD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="1960" windowWidth="25880" windowHeight="17920" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="460" windowWidth="32380" windowHeight="24640" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="salinity" sheetId="6" r:id="rId1"/>
@@ -18659,8 +18659,8 @@
   </sheetPr>
   <dimension ref="A1:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -19214,14 +19214,14 @@
         <v>2264.1765586140868</v>
       </c>
       <c r="Y10" s="73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z10" s="148">
         <f>nuts!AB4</f>
         <v>2188.4771117615464</v>
       </c>
       <c r="AA10" s="73">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
@@ -19295,14 +19295,14 @@
         <v>2252.9593465639464</v>
       </c>
       <c r="Y11" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z11" s="148">
         <f>nuts!AB5</f>
         <v>2176.6924075719849</v>
       </c>
       <c r="AA11" s="73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB11" s="71"/>
       <c r="AC11" s="71"/>
@@ -19378,7 +19378,7 @@
         <v>2148.243613799018</v>
       </c>
       <c r="Y12" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z12" s="148">
         <f>nuts!AB6</f>
@@ -19461,7 +19461,7 @@
         <v>2110.6957798261783</v>
       </c>
       <c r="Y13" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z13" s="148">
         <f>nuts!AB7</f>
@@ -19544,14 +19544,14 @@
         <v>2257.2644278770172</v>
       </c>
       <c r="Y14" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z14" s="148">
         <f>nuts!AB8</f>
         <v>2152.7228091704651</v>
       </c>
       <c r="AA14" s="73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB14" s="71"/>
       <c r="AC14" s="71"/>
@@ -19627,14 +19627,14 @@
         <v>2263.2537845141587</v>
       </c>
       <c r="Y15" s="73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z15" s="148">
         <f>nuts!AB9</f>
         <v>2150.3712870853251</v>
       </c>
       <c r="AA15" s="73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB15" s="71"/>
       <c r="AC15" s="71"/>
@@ -19710,14 +19710,14 @@
         <v>2243.4924357873088</v>
       </c>
       <c r="Y16" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z16" s="148">
         <f>nuts!AB10</f>
         <v>2154.4058306871457</v>
       </c>
       <c r="AA16" s="73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB16" s="71"/>
       <c r="AC16" s="71"/>
@@ -19799,7 +19799,7 @@
         <v>2174.3445516244706</v>
       </c>
       <c r="AA17" s="73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB17" s="71"/>
       <c r="AC17" s="71"/>
@@ -19875,14 +19875,14 @@
         <v>2281.4200589017091</v>
       </c>
       <c r="Y18" s="73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z18" s="148">
         <f>nuts!AB12</f>
         <v>2178.1344507717508</v>
       </c>
       <c r="AA18" s="73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB18" s="71"/>
       <c r="AC18" s="71"/>
@@ -20036,7 +20036,7 @@
         <v>2178.1625516318886</v>
       </c>
       <c r="Y20" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z20" s="148">
         <f>nuts!AB14</f>
@@ -20119,7 +20119,7 @@
         <v>2281.274719263854</v>
       </c>
       <c r="Y21" s="73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z21" s="148">
         <f>nuts!AB15</f>
@@ -20202,7 +20202,7 @@
         <v>2285.4800595568272</v>
       </c>
       <c r="Y22" s="73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z22" s="148">
         <f>nuts!AB16</f>
@@ -20285,7 +20285,7 @@
         <v>2174.3144103220552</v>
       </c>
       <c r="Y23" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z23" s="148">
         <f>nuts!AB17</f>
@@ -20368,7 +20368,7 @@
         <v>2191.593965183753</v>
       </c>
       <c r="Y24" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z24" s="148">
         <f>nuts!AB18</f>
@@ -20451,7 +20451,7 @@
         <v>2180.9742782106277</v>
       </c>
       <c r="Y25" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z25" s="148">
         <f>nuts!AB19</f>
@@ -20534,7 +20534,7 @@
         <v>2198.686328517736</v>
       </c>
       <c r="Y26" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z26" s="148">
         <f>nuts!AB20</f>
@@ -20617,7 +20617,7 @@
         <v>2244.5267642665071</v>
       </c>
       <c r="Y27" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z27" s="148">
         <f>nuts!AB21</f>
@@ -20700,7 +20700,7 @@
         <v>2184.8730098745118</v>
       </c>
       <c r="Y28" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z28" s="148">
         <f>nuts!AB22</f>
@@ -20783,7 +20783,7 @@
         <v>2149.7982621746437</v>
       </c>
       <c r="Y29" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z29" s="148">
         <f>nuts!AB23</f>
@@ -20866,7 +20866,7 @@
         <v>2222.5265207003517</v>
       </c>
       <c r="Y30" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z30" s="148">
         <f>nuts!AB24</f>
@@ -20949,7 +20949,7 @@
         <v>2232.4239537363333</v>
       </c>
       <c r="Y31" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z31" s="148">
         <f>nuts!AB25</f>
@@ -21032,14 +21032,14 @@
         <v>2189.1993111466099</v>
       </c>
       <c r="Y32" s="73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z32" s="148">
         <f>nuts!AB26</f>
         <v>2046.1655673491657</v>
       </c>
       <c r="AA32" s="73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB32" s="71"/>
       <c r="AC32" s="71"/>

</xml_diff>